<commit_message>
add missing organization/role property
</commit_message>
<xml_diff>
--- a/fictional-example/flattened/ocds-213czf-000-00001-01-planning.xlsx
+++ b/fictional-example/flattened/ocds-213czf-000-00001-01-planning.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="315">
   <si>
     <t>ocid</t>
   </si>
@@ -43,66 +43,66 @@
     <t>id</t>
   </si>
   <si>
+    <t>parties/0/id</t>
+  </si>
+  <si>
+    <t>parties/0/name</t>
+  </si>
+  <si>
     <t>language</t>
   </si>
   <si>
+    <t>parties/0/roles</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
-    <t>parties/0/id</t>
-  </si>
-  <si>
     <t>initiationType</t>
   </si>
   <si>
-    <t>parties/0/name</t>
+    <t>parties/0/identifier/scheme</t>
   </si>
   <si>
     <t>tag</t>
   </si>
   <si>
-    <t>parties/0/roles</t>
+    <t>parties/0/identifier/id</t>
+  </si>
+  <si>
+    <t>parties/0/identifier/legalName</t>
   </si>
   <si>
     <t>ocds-213czf-000-00001</t>
   </si>
   <si>
+    <t>parties/0/identifier/uri</t>
+  </si>
+  <si>
     <t>ocds-213czf-000-00001-01-planning</t>
   </si>
   <si>
+    <t>parties/0/address/streetAddress</t>
+  </si>
+  <si>
     <t>en</t>
   </si>
   <si>
+    <t>parties/0/address/locality</t>
+  </si>
+  <si>
     <t>2009-03-15T14:45:00Z</t>
   </si>
   <si>
+    <t>parties/0/address/region</t>
+  </si>
+  <si>
     <t>tender</t>
   </si>
   <si>
     <t>planning</t>
   </si>
   <si>
-    <t>parties/0/identifier/scheme</t>
-  </si>
-  <si>
-    <t>parties/0/identifier/id</t>
-  </si>
-  <si>
-    <t>parties/0/identifier/legalName</t>
-  </si>
-  <si>
-    <t>parties/0/identifier/uri</t>
-  </si>
-  <si>
-    <t>parties/0/address/streetAddress</t>
-  </si>
-  <si>
-    <t>parties/0/address/locality</t>
-  </si>
-  <si>
-    <t>parties/0/address/region</t>
-  </si>
-  <si>
     <t>parties/0/address/postalCode</t>
   </si>
   <si>
@@ -130,6 +130,9 @@
     <t>London Borough of Barnet</t>
   </si>
   <si>
+    <t>buyer</t>
+  </si>
+  <si>
     <t>GB-LAC</t>
   </si>
   <si>
@@ -160,15 +163,15 @@
     <t>01234 345 345</t>
   </si>
   <si>
+    <t>buyer/id</t>
+  </si>
+  <si>
+    <t>buyer/name</t>
+  </si>
+  <si>
     <t>http://example.com/contact/</t>
   </si>
   <si>
-    <t>buyer/id</t>
-  </si>
-  <si>
-    <t>buyer/name</t>
-  </si>
-  <si>
     <t>planning/budget/id</t>
   </si>
   <si>
@@ -193,24 +196,24 @@
     <t>planning/rationale</t>
   </si>
   <si>
+    <t>planning/documents/0/id</t>
+  </si>
+  <si>
+    <t>planning/documents/0/documentType</t>
+  </si>
+  <si>
     <t>6801ad388f3a38b7740dde20108c58b35984ee91</t>
   </si>
   <si>
+    <t>planning/documents/0/title</t>
+  </si>
+  <si>
+    <t>planning/documents/0/description</t>
+  </si>
+  <si>
     <t xml:space="preserve">Budget allocation for highway maintenance, aligned with 2015 strategic plan. </t>
   </si>
   <si>
-    <t>planning/documents/0/id</t>
-  </si>
-  <si>
-    <t>planning/documents/0/documentType</t>
-  </si>
-  <si>
-    <t>planning/documents/0/title</t>
-  </si>
-  <si>
-    <t>planning/documents/0/description</t>
-  </si>
-  <si>
     <t>planning/documents/0/url</t>
   </si>
   <si>
@@ -232,12 +235,12 @@
     <t>procurementPlan</t>
   </si>
   <si>
+    <t>Area Wide Cycle Improvements - Procurement Plan</t>
+  </si>
+  <si>
     <t>Central Junction Cycle Scheme</t>
   </si>
   <si>
-    <t>Area Wide Cycle Improvements - Procurement Plan</t>
-  </si>
-  <si>
     <t>SP001</t>
   </si>
   <si>
@@ -259,48 +262,48 @@
     <t>application/pdf</t>
   </si>
   <si>
+    <t>planning/milestones/0/id</t>
+  </si>
+  <si>
+    <t>planning/milestones/0/type</t>
+  </si>
+  <si>
+    <t>planning/milestones/0/code</t>
+  </si>
+  <si>
+    <t>planning/milestones/0/title</t>
+  </si>
+  <si>
     <t>needsAssessment</t>
   </si>
   <si>
+    <t>planning/milestones/0/description</t>
+  </si>
+  <si>
     <t>Cycle provision - Needs Assessment</t>
   </si>
   <si>
+    <t>planning/milestones/0/status</t>
+  </si>
+  <si>
     <t>Needs assessment for provision for cyclists in the centre of town.</t>
   </si>
   <si>
+    <t>planning/milestones/0/dueDate</t>
+  </si>
+  <si>
+    <t>planning/milestones/0/dateMet</t>
+  </si>
+  <si>
     <t>http://example.com/opencontracting/documents/ocds-213czf-000-00001/needsAssessment.pdf</t>
   </si>
   <si>
+    <t>planning/milestones/0/dateModified</t>
+  </si>
+  <si>
     <t>2009-01-15T00:00:00Z</t>
   </si>
   <si>
-    <t>planning/milestones/0/id</t>
-  </si>
-  <si>
-    <t>planning/milestones/0/type</t>
-  </si>
-  <si>
-    <t>planning/milestones/0/code</t>
-  </si>
-  <si>
-    <t>planning/milestones/0/title</t>
-  </si>
-  <si>
-    <t>planning/milestones/0/description</t>
-  </si>
-  <si>
-    <t>planning/milestones/0/status</t>
-  </si>
-  <si>
-    <t>planning/milestones/0/dueDate</t>
-  </si>
-  <si>
-    <t>planning/milestones/0/dateMet</t>
-  </si>
-  <si>
-    <t>planning/milestones/0/dateModified</t>
-  </si>
-  <si>
     <t>preProcurement</t>
   </si>
   <si>
@@ -337,174 +340,174 @@
     <t>tender/title</t>
   </si>
   <si>
+    <t>tender/description</t>
+  </si>
+  <si>
+    <t>tender/mainProcurementCategory</t>
+  </si>
+  <si>
+    <t>tender/status</t>
+  </si>
+  <si>
+    <t>tender/minValue/amount</t>
+  </si>
+  <si>
+    <t>tender/minValue/currency</t>
+  </si>
+  <si>
+    <t>tender/value/amount</t>
+  </si>
+  <si>
+    <t>tender/value/currency</t>
+  </si>
+  <si>
+    <t>tender/procurementMethod</t>
+  </si>
+  <si>
+    <t>tender/procurementMethodDetails</t>
+  </si>
+  <si>
+    <t>tender/procurementMethodRationale</t>
+  </si>
+  <si>
     <t>tender/documents/0/id</t>
   </si>
   <si>
-    <t>tender/description</t>
+    <t>tender/awardCriteria</t>
   </si>
   <si>
     <t>tender/documents/0/documentType</t>
   </si>
   <si>
-    <t>tender/mainProcurementCategory</t>
+    <t>tender/awardCriteriaDetails</t>
   </si>
   <si>
     <t>tender/documents/0/title</t>
   </si>
   <si>
-    <t>tender/status</t>
-  </si>
-  <si>
-    <t>tender/minValue/amount</t>
+    <t>tender/tenderers/0/id</t>
+  </si>
+  <si>
+    <t>tender/submissionMethod</t>
   </si>
   <si>
     <t>tender/documents/0/description</t>
   </si>
   <si>
-    <t>tender/minValue/currency</t>
+    <t>tender/tenderers/0/name</t>
   </si>
   <si>
     <t>tender/documents/0/url</t>
   </si>
   <si>
+    <t>tender/submissionMethodDetails</t>
+  </si>
+  <si>
     <t>tender/documents/0/datePublished</t>
   </si>
   <si>
-    <t>tender/value/amount</t>
-  </si>
-  <si>
-    <t>tender/value/currency</t>
+    <t>tender/tenderPeriod/startDate</t>
   </si>
   <si>
     <t>tender/documents/0/dateModified</t>
   </si>
   <si>
-    <t>tender/procurementMethod</t>
+    <t>tender/tenderPeriod/endDate</t>
   </si>
   <si>
     <t>tender/documents/0/format</t>
   </si>
   <si>
-    <t>tender/procurementMethodDetails</t>
-  </si>
-  <si>
     <t>tender/documents/0/language</t>
   </si>
   <si>
-    <t>tender/procurementMethodRationale</t>
-  </si>
-  <si>
-    <t>tender/awardCriteria</t>
-  </si>
-  <si>
-    <t>tender/awardCriteriaDetails</t>
-  </si>
-  <si>
-    <t>tender/submissionMethod</t>
-  </si>
-  <si>
-    <t>tender/submissionMethodDetails</t>
+    <t>tender/tenderPeriod/durationInDays</t>
+  </si>
+  <si>
+    <t>tender/enquiryPeriod/startDate</t>
+  </si>
+  <si>
+    <t>tender/enquiryPeriod/endDate</t>
+  </si>
+  <si>
+    <t>tender/enquiryPeriod/durationInDays</t>
   </si>
   <si>
     <t>x_consultationDocument</t>
   </si>
   <si>
-    <t>tender/tenderPeriod/startDate</t>
+    <t>tender/eligibilityCriteria</t>
   </si>
   <si>
     <t>Consultation on cycle provision</t>
   </si>
   <si>
-    <t>tender/tenderPeriod/endDate</t>
-  </si>
-  <si>
-    <t>tender/tenderPeriod/durationInDays</t>
+    <t>tender/awardPeriod/startDate</t>
+  </si>
+  <si>
+    <t>tender/awardPeriod/endDate</t>
   </si>
   <si>
     <t>A consultation document inviting citizen input into cycle provision.</t>
   </si>
   <si>
-    <t>tender/enquiryPeriod/startDate</t>
+    <t>tender/contractPeriod/startDate</t>
+  </si>
+  <si>
+    <t>tender/contractPeriod/endDate</t>
   </si>
   <si>
     <t>http://example.com/consultations/cycle-provision/</t>
   </si>
   <si>
-    <t>tender/enquiryPeriod/endDate</t>
-  </si>
-  <si>
-    <t>tender/enquiryPeriod/durationInDays</t>
-  </si>
-  <si>
-    <t>tender/eligibilityCriteria</t>
+    <t>tender/contractPeriod/durationInDays</t>
+  </si>
+  <si>
+    <t>tender/procuringEntity/id</t>
+  </si>
+  <si>
+    <t>tender/procuringEntity/name</t>
+  </si>
+  <si>
+    <t>tender/numberOfTenderers</t>
+  </si>
+  <si>
+    <t>tender/hasEnquiries</t>
   </si>
   <si>
     <t>2010-02-15T00:00:00Z</t>
   </si>
   <si>
-    <t>tender/awardPeriod/startDate</t>
-  </si>
-  <si>
     <t>text/html</t>
   </si>
   <si>
-    <t>tender/awardPeriod/endDate</t>
-  </si>
-  <si>
-    <t>tender/contractPeriod/startDate</t>
-  </si>
-  <si>
-    <t>tender/contractPeriod/endDate</t>
+    <t>Planned cycle lane improvements</t>
   </si>
   <si>
     <t>x_map</t>
   </si>
   <si>
-    <t>tender/contractPeriod/durationInDays</t>
+    <t>The authority plans to tender for improvements to the cycle lane in early 2010. This notice provides advanced notice of the intention to tender, and details to upcoming consultation events.</t>
   </si>
   <si>
     <t>Map of affected areas</t>
   </si>
   <si>
-    <t>tender/procuringEntity/id</t>
+    <t>works</t>
+  </si>
+  <si>
+    <t>planned</t>
   </si>
   <si>
     <t>A map showing areas affected by the planned highway updates. Available from local libraries.</t>
   </si>
   <si>
-    <t>tender/procuringEntity/name</t>
-  </si>
-  <si>
-    <t>tender/numberOfTenderers</t>
-  </si>
-  <si>
     <t>offline/print</t>
   </si>
   <si>
-    <t>tender/hasEnquiries</t>
-  </si>
-  <si>
-    <t>Planned cycle lane improvements</t>
-  </si>
-  <si>
-    <t>The authority plans to tender for improvements to the cycle lane in early 2010. This notice provides advanced notice of the intention to tender, and details to upcoming consultation events.</t>
-  </si>
-  <si>
-    <t>works</t>
-  </si>
-  <si>
-    <t>planned</t>
-  </si>
-  <si>
-    <t>tender/tenderers/0/id</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
-    <t>tender/tenderers/0/name</t>
-  </si>
-  <si>
     <t xml:space="preserve">In open procedures, any interested economic operator may submit a tender in response to a contract notice. </t>
   </si>
   <si>
@@ -553,66 +556,66 @@
     <t>tender/items/0/unit/id</t>
   </si>
   <si>
+    <t>tender/items/0/unit/scheme</t>
+  </si>
+  <si>
+    <t>tender/items/0/unit/uri</t>
+  </si>
+  <si>
+    <t>tender/items/0/unit/value/amount</t>
+  </si>
+  <si>
+    <t>tender/items/0/unit/value/currency</t>
+  </si>
+  <si>
+    <t>Cycle lane improvements</t>
+  </si>
+  <si>
+    <t>CPV</t>
+  </si>
+  <si>
+    <t>Construction work for highways</t>
+  </si>
+  <si>
+    <t>http://cpv.data.ac.uk/code-45233130</t>
+  </si>
+  <si>
     <t>tender/items/0/additionalClassifications/0/scheme</t>
   </si>
   <si>
-    <t>tender/items/0/unit/scheme</t>
-  </si>
-  <si>
     <t>tender/items/0/additionalClassifications/0/id</t>
   </si>
   <si>
     <t>tender/items/0/additionalClassifications/0/description</t>
   </si>
   <si>
-    <t>tender/items/0/unit/uri</t>
+    <t>Miles</t>
   </si>
   <si>
     <t>tender/items/0/additionalClassifications/0/uri</t>
   </si>
   <si>
-    <t>tender/items/0/unit/value/amount</t>
-  </si>
-  <si>
-    <t>tender/items/0/unit/value/currency</t>
-  </si>
-  <si>
-    <t>CPV</t>
+    <t>SMI</t>
+  </si>
+  <si>
+    <t>UNCEFACT</t>
   </si>
   <si>
     <t>45233162-2</t>
   </si>
   <si>
+    <t>tender/amendments/0/date</t>
+  </si>
+  <si>
     <t>Cycle path construction work</t>
   </si>
   <si>
+    <t>tender/amendments/0/rationale</t>
+  </si>
+  <si>
     <t>http://cpv.data.ac.uk/code-45233162.html</t>
   </si>
   <si>
-    <t>Cycle lane improvements</t>
-  </si>
-  <si>
-    <t>Construction work for highways</t>
-  </si>
-  <si>
-    <t>http://cpv.data.ac.uk/code-45233130</t>
-  </si>
-  <si>
-    <t>Miles</t>
-  </si>
-  <si>
-    <t>SMI</t>
-  </si>
-  <si>
-    <t>UNCEFACT</t>
-  </si>
-  <si>
-    <t>tender/amendments/0/date</t>
-  </si>
-  <si>
-    <t>tender/amendments/0/rationale</t>
-  </si>
-  <si>
     <t>tender/amendments/0/id</t>
   </si>
   <si>
@@ -631,141 +634,141 @@
     <t>awards/0/title</t>
   </si>
   <si>
+    <t>awards/0/items/0/id</t>
+  </si>
+  <si>
     <t>awards/0/description</t>
   </si>
   <si>
+    <t>awards/0/items/0/description</t>
+  </si>
+  <si>
     <t>awards/0/status</t>
   </si>
   <si>
+    <t>awards/0/items/0/classification/scheme</t>
+  </si>
+  <si>
     <t>awards/0/date</t>
   </si>
   <si>
+    <t>awards/0/items/0/classification/id</t>
+  </si>
+  <si>
     <t>awards/0/value/amount</t>
   </si>
   <si>
+    <t>awards/0/items/0/classification/description</t>
+  </si>
+  <si>
     <t>awards/0/value/currency</t>
   </si>
   <si>
     <t>awards/0/suppliers/0/id</t>
   </si>
   <si>
+    <t>awards/0/items/0/classification/uri</t>
+  </si>
+  <si>
     <t>awards/0/suppliers/0/name</t>
   </si>
   <si>
+    <t>awards/0/items/0/quantity</t>
+  </si>
+  <si>
     <t>awards/0/contractPeriod/startDate</t>
   </si>
   <si>
+    <t>awards/0/items/0/unit/name</t>
+  </si>
+  <si>
     <t>awards/0/contractPeriod/endDate</t>
   </si>
   <si>
+    <t>awards/0/items/0/additionalClassifications/0/scheme</t>
+  </si>
+  <si>
+    <t>awards/0/items/0/unit/id</t>
+  </si>
+  <si>
     <t>awards/0/contractPeriod/maxExtentDate</t>
   </si>
   <si>
+    <t>awards/0/items/0/unit/scheme</t>
+  </si>
+  <si>
+    <t>awards/0/items/0/additionalClassifications/0/id</t>
+  </si>
+  <si>
     <t>awards/0/contractPeriod/durationInDays</t>
   </si>
   <si>
-    <t>awards/0/items/0/id</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/description</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/classification/scheme</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/classification/id</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/classification/description</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/classification/uri</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/quantity</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/unit/name</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/unit/id</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/unit/scheme</t>
-  </si>
-  <si>
-    <t>awards/0/items/0/additionalClassifications/0/scheme</t>
-  </si>
-  <si>
     <t>awards/0/items/0/unit/uri</t>
   </si>
   <si>
+    <t>awards/0/items/0/additionalClassifications/0/description</t>
+  </si>
+  <si>
     <t>awards/0/items/0/unit/value/amount</t>
   </si>
   <si>
-    <t>awards/0/items/0/additionalClassifications/0/id</t>
-  </si>
-  <si>
     <t>awards/0/items/0/unit/value/currency</t>
   </si>
   <si>
-    <t>awards/0/items/0/additionalClassifications/0/description</t>
-  </si>
-  <si>
     <t>awards/0/items/0/additionalClassifications/0/uri</t>
   </si>
   <si>
     <t>awards/0/documents/0/id</t>
   </si>
   <si>
+    <t>contracts/0/id</t>
+  </si>
+  <si>
     <t>awards/0/documents/0/documentType</t>
   </si>
   <si>
+    <t>contracts/0/awardID</t>
+  </si>
+  <si>
     <t>awards/0/documents/0/title</t>
   </si>
   <si>
     <t>awards/0/documents/0/description</t>
   </si>
   <si>
+    <t>contracts/0/title</t>
+  </si>
+  <si>
     <t>awards/0/documents/0/url</t>
   </si>
   <si>
+    <t>contracts/0/description</t>
+  </si>
+  <si>
     <t>awards/0/documents/0/datePublished</t>
   </si>
   <si>
+    <t>contracts/0/status</t>
+  </si>
+  <si>
     <t>awards/0/documents/0/dateModified</t>
   </si>
   <si>
+    <t>contracts/0/period/startDate</t>
+  </si>
+  <si>
+    <t>contracts/0/period/endDate</t>
+  </si>
+  <si>
     <t>awards/0/documents/0/format</t>
   </si>
   <si>
+    <t>contracts/0/period/maxExtentDate</t>
+  </si>
+  <si>
     <t>awards/0/documents/0/language</t>
   </si>
   <si>
-    <t>contracts/0/id</t>
-  </si>
-  <si>
-    <t>contracts/0/awardID</t>
-  </si>
-  <si>
-    <t>contracts/0/title</t>
-  </si>
-  <si>
-    <t>contracts/0/description</t>
-  </si>
-  <si>
-    <t>contracts/0/status</t>
-  </si>
-  <si>
-    <t>contracts/0/period/startDate</t>
-  </si>
-  <si>
-    <t>contracts/0/period/endDate</t>
-  </si>
-  <si>
-    <t>contracts/0/period/maxExtentDate</t>
-  </si>
-  <si>
     <t>contracts/0/period/durationInDays</t>
   </si>
   <si>
@@ -817,28 +820,28 @@
     <t>contracts/0/items/0/unit/value/currency</t>
   </si>
   <si>
+    <t>contracts/0/relatedProcesses/0/id</t>
+  </si>
+  <si>
     <t>contracts/0/items/0/additionalClassifications/0/scheme</t>
   </si>
   <si>
+    <t>contracts/0/relatedProcesses/0/title</t>
+  </si>
+  <si>
     <t>contracts/0/items/0/additionalClassifications/0/id</t>
   </si>
   <si>
+    <t>contracts/0/relatedProcesses/0/relationship</t>
+  </si>
+  <si>
     <t>contracts/0/items/0/additionalClassifications/0/description</t>
   </si>
   <si>
+    <t>contracts/0/relatedProcesses/0/scheme</t>
+  </si>
+  <si>
     <t>contracts/0/items/0/additionalClassifications/0/uri</t>
-  </si>
-  <si>
-    <t>contracts/0/relatedProcesses/0/id</t>
-  </si>
-  <si>
-    <t>contracts/0/relatedProcesses/0/title</t>
-  </si>
-  <si>
-    <t>contracts/0/relatedProcesses/0/relationship</t>
-  </si>
-  <si>
-    <t>contracts/0/relatedProcesses/0/scheme</t>
   </si>
   <si>
     <t>contracts/0/relatedProcesses/0/identifier</t>
@@ -1174,10 +1177,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>155</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1200,87 +1203,87 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>173</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F2" s="3">
         <v>4.523313E7</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="I2" s="3">
         <v>10.0</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="N2" s="3">
         <v>100000.0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1306,42 +1309,42 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -1367,22 +1370,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>191</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1405,43 +1408,43 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1464,46 +1467,46 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>216</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>217</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -1526,22 +1529,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -1564,34 +1567,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>232</v>
+        <v>238</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -1614,40 +1617,40 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>242</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -1670,46 +1673,46 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -1732,36 +1735,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1784,22 +1787,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -1822,25 +1825,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>266</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>267</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1863,34 +1866,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -1913,37 +1916,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -1966,34 +1969,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -2013,7 +2016,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B1" s="5">
         <v>1.1</v>
@@ -2021,44 +2024,44 @@
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B7" s="1">
         <v>9506232.0</v>
@@ -2066,26 +2069,26 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -2114,34 +2117,34 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>22</v>
@@ -2167,10 +2170,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>29</v>
@@ -2178,44 +2181,47 @@
       <c r="D2" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2249,10 +2255,10 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>29</v>
@@ -2281,60 +2287,60 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="E2" s="3">
         <v>6700000.0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -2360,10 +2366,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>56</v>
@@ -2372,83 +2378,83 @@
         <v>57</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -2475,28 +2481,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>87</v>
@@ -2504,57 +2510,57 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>1.0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3">
         <v>2.0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2577,70 +2583,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="Q1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="S1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>129</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>132</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>133</v>
@@ -2649,7 +2655,7 @@
         <v>135</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>138</v>
@@ -2661,69 +2667,69 @@
         <v>141</v>
       </c>
       <c r="AE1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>150</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H2" s="3">
         <v>500000.0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J2" s="3">
         <v>1000000.0</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="U2" s="3">
         <v>31.0</v>
@@ -2732,10 +2738,10 @@
         <v>14.0</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AD2" s="3">
         <v>365.0</v>
@@ -2767,92 +2773,92 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>3.0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3">
         <v>4.0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>